<commit_message>
Add Soroban operation generators and configuration files
Added multiple Python scripts for generating Soroban sum and subtraction exercises (generator.py, main.py, nuevo codigo.py, flash_anzan2.py, rules.py), configuration file (config.json), and supporting Excel files for operation rules and weights. Also updated flash_anzan.py and flash_anzan.xlsx with minor changes. These additions enable flexible generation and export of Soroban practice problems based on configurable steps and rules.
</commit_message>
<xml_diff>
--- a/flash_anzan.xlsx
+++ b/flash_anzan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c8a8fd3e0d48bb0/Documentos 1/Documentos/ELAB/Soroban/Codigos/flash_anzan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7115" documentId="8_{9B207387-4476-428A-8A5E-83DE628ABDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50955CEB-EF17-40FB-80D1-14C81347BF72}"/>
+  <xr:revisionPtr revIDLastSave="20859" documentId="8_{9B207387-4476-428A-8A5E-83DE628ABDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BACF061-26D6-46EB-95B2-F62C7C74940C}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-2475" windowWidth="29040" windowHeight="15840" xr2:uid="{0C39B2B9-CE23-4F52-9F9D-FE743E645FE8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0C39B2B9-CE23-4F52-9F9D-FE743E645FE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
     <t>Resultado</t>
   </si>
   <si>
-    <t>[43, -40, 9, -5, 58, -38]</t>
+    <t>[48, -47, -1, 23, 21, 5]</t>
   </si>
 </sst>
 </file>
@@ -116,13 +116,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,6 +159,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -191,6 +197,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -200,8 +208,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -256,9 +262,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
+      <xdr:colOff>708058</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>126143</xdr:rowOff>
+      <xdr:rowOff>136444</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -289,7 +295,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="695325" cy="697643"/>
+          <a:ext cx="711868" cy="681675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -678,103 +684,104 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC9A00F-2CB1-479C-9533-01F728982785}">
   <dimension ref="B4:K12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="4">
         <v>2</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
-    <row r="7" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="4">
-        <v>8</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="4">
         <v>5</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="C10" s="5">
-        <v>27</v>
-      </c>
-      <c r="D10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="6">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C12" s="7" t="str">
         <f>+IF(C11=C10, "CORRECTO","MAL")</f>
         <v>CORRECTO</v>

</xml_diff>